<commit_message>
Add unit test and update BL
</commit_message>
<xml_diff>
--- a/PowerPlantCodingChallenge/UnitTest/Engie Coding Challenge.xlsx
+++ b/PowerPlantCodingChallenge/UnitTest/Engie Coding Challenge.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryan\Documents\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Personal Projects\powerplant-coding-challenge\PowerPlantCodingChallenge\UnitTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38202171-CE39-4999-8236-59ACC053C233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0415E2A-C0F0-4759-B7D1-A649658BB20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{ED8C14AC-36C7-4E71-8B40-32367028DD95}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -116,6 +116,42 @@
   </si>
   <si>
     <t>Payload 4</t>
+  </si>
+  <si>
+    <t>Payload 5</t>
+  </si>
+  <si>
+    <t>Payload 6</t>
+  </si>
+  <si>
+    <t>LOAD : 183,6</t>
+  </si>
+  <si>
+    <t>Payload 7</t>
+  </si>
+  <si>
+    <t>LOAD : 173,6</t>
+  </si>
+  <si>
+    <t>Payload 8</t>
+  </si>
+  <si>
+    <t>LOAD : 71,6</t>
+  </si>
+  <si>
+    <t>LOAD : 86,6</t>
+  </si>
+  <si>
+    <t>LOAD : 31,6</t>
+  </si>
+  <si>
+    <t>LOAD : 152</t>
+  </si>
+  <si>
+    <t>Payload 9</t>
+  </si>
+  <si>
+    <t>Payload 10</t>
   </si>
 </sst>
 </file>
@@ -299,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -323,9 +359,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -718,7 +751,7 @@
       <c r="H5" s="6">
         <v>0.53</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="15">
         <f xml:space="preserve"> G5 / H5</f>
         <v>25.283018867924529</v>
       </c>
@@ -728,16 +761,16 @@
       <c r="E6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="9">
+      <c r="F6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="4">
         <v>13.4</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="4">
         <v>0.53</v>
       </c>
-      <c r="I6" s="17">
+      <c r="I6" s="16">
         <f xml:space="preserve"> G6 / H6</f>
         <v>25.283018867924529</v>
       </c>
@@ -747,16 +780,16 @@
       <c r="E7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="9">
+      <c r="F7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="4">
         <v>13.4</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="4">
         <v>0.37</v>
       </c>
-      <c r="I7" s="17">
+      <c r="I7" s="16">
         <f xml:space="preserve"> G7 / H7</f>
         <v>36.216216216216218</v>
       </c>
@@ -766,16 +799,16 @@
       <c r="E8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="4">
         <v>50.8</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="4">
         <v>0.3</v>
       </c>
-      <c r="I8" s="17">
+      <c r="I8" s="16">
         <f t="shared" ref="I8:I10" si="0" xml:space="preserve"> G8 / H8</f>
         <v>169.33333333333334</v>
       </c>
@@ -785,35 +818,35 @@
       <c r="E9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="9">
-        <v>0</v>
-      </c>
-      <c r="H9" s="9">
-        <v>1</v>
-      </c>
-      <c r="I9" s="17">
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1</v>
+      </c>
+      <c r="I9" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="4:9" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D10" s="4"/>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="12">
-        <v>0</v>
-      </c>
-      <c r="H10" s="12">
-        <v>1</v>
-      </c>
-      <c r="I10" s="18">
+      <c r="G10" s="11">
+        <v>0</v>
+      </c>
+      <c r="H10" s="11">
+        <v>1</v>
+      </c>
+      <c r="I10" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -870,13 +903,13 @@
       <c r="F15" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="4">
         <v>13.4</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="4">
         <v>0.53</v>
       </c>
-      <c r="I15" s="16">
+      <c r="I15" s="15">
         <f xml:space="preserve"> G15 / H15</f>
         <v>25.283018867924529</v>
       </c>
@@ -886,16 +919,16 @@
       <c r="E16" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="9">
+      <c r="F16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="4">
         <v>13.4</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="4">
         <v>0.53</v>
       </c>
-      <c r="I16" s="17">
+      <c r="I16" s="16">
         <f xml:space="preserve"> G16 / H16</f>
         <v>25.283018867924529</v>
       </c>
@@ -905,16 +938,16 @@
       <c r="E17" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" s="9">
+      <c r="F17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="4">
         <v>13.4</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H17" s="4">
         <v>0.37</v>
       </c>
-      <c r="I17" s="17">
+      <c r="I17" s="16">
         <f xml:space="preserve"> G17 / H17</f>
         <v>36.216216216216218</v>
       </c>
@@ -924,16 +957,16 @@
       <c r="E18" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="4">
         <v>50.8</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="4">
         <v>0.3</v>
       </c>
-      <c r="I18" s="17">
+      <c r="I18" s="16">
         <f t="shared" ref="I18:I20" si="1" xml:space="preserve"> G18 / H18</f>
         <v>169.33333333333334</v>
       </c>
@@ -943,35 +976,35 @@
       <c r="E19" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="9">
-        <v>0</v>
-      </c>
-      <c r="H19" s="9">
-        <v>1</v>
-      </c>
-      <c r="I19" s="17">
+      <c r="G19" s="4">
+        <v>0</v>
+      </c>
+      <c r="H19" s="4">
+        <v>1</v>
+      </c>
+      <c r="I19" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="4:9" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D20" s="4"/>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="12">
-        <v>0</v>
-      </c>
-      <c r="H20" s="12">
-        <v>1</v>
-      </c>
-      <c r="I20" s="18">
+      <c r="G20" s="11">
+        <v>0</v>
+      </c>
+      <c r="H20" s="11">
+        <v>1</v>
+      </c>
+      <c r="I20" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1028,13 +1061,13 @@
       <c r="F25" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G25" s="9">
+      <c r="G25" s="4">
         <v>13.4</v>
       </c>
-      <c r="H25" s="9">
+      <c r="H25" s="4">
         <v>0.53</v>
       </c>
-      <c r="I25" s="16">
+      <c r="I25" s="15">
         <f xml:space="preserve"> G25 / H25</f>
         <v>25.283018867924529</v>
       </c>
@@ -1044,16 +1077,16 @@
       <c r="E26" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="9">
+      <c r="F26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="4">
         <v>13.4</v>
       </c>
-      <c r="H26" s="9">
+      <c r="H26" s="4">
         <v>0.53</v>
       </c>
-      <c r="I26" s="17">
+      <c r="I26" s="16">
         <f xml:space="preserve"> G26 / H26</f>
         <v>25.283018867924529</v>
       </c>
@@ -1063,16 +1096,16 @@
       <c r="E27" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" s="9">
+      <c r="F27" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="4">
         <v>13.4</v>
       </c>
-      <c r="H27" s="9">
+      <c r="H27" s="4">
         <v>0.37</v>
       </c>
-      <c r="I27" s="17">
+      <c r="I27" s="16">
         <f xml:space="preserve"> G27 / H27</f>
         <v>36.216216216216218</v>
       </c>
@@ -1082,16 +1115,16 @@
       <c r="E28" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F28" s="9" t="s">
+      <c r="F28" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G28" s="9">
+      <c r="G28" s="4">
         <v>50.8</v>
       </c>
-      <c r="H28" s="9">
+      <c r="H28" s="4">
         <v>0.3</v>
       </c>
-      <c r="I28" s="17">
+      <c r="I28" s="16">
         <f t="shared" ref="I28:I30" si="2" xml:space="preserve"> G28 / H28</f>
         <v>169.33333333333334</v>
       </c>
@@ -1101,35 +1134,35 @@
       <c r="E29" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="9" t="s">
+      <c r="F29" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G29" s="9">
-        <v>0</v>
-      </c>
-      <c r="H29" s="9">
-        <v>1</v>
-      </c>
-      <c r="I29" s="17">
+      <c r="G29" s="4">
+        <v>0</v>
+      </c>
+      <c r="H29" s="4">
+        <v>1</v>
+      </c>
+      <c r="I29" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="4:9" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D30" s="4"/>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F30" s="12" t="s">
+      <c r="F30" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G30" s="12">
-        <v>0</v>
-      </c>
-      <c r="H30" s="12">
-        <v>1</v>
-      </c>
-      <c r="I30" s="18">
+      <c r="G30" s="11">
+        <v>0</v>
+      </c>
+      <c r="H30" s="11">
+        <v>1</v>
+      </c>
+      <c r="I30" s="17">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1142,10 +1175,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66881AD8-C236-45BB-A40E-8E5D21E48D9A}">
-  <dimension ref="C3:L40"/>
+  <dimension ref="C3:L95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="I86" sqref="I86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1166,7 +1199,7 @@
       <c r="L3" s="4"/>
     </row>
     <row r="4" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -1213,8 +1246,8 @@
       <c r="I5" s="5">
         <v>150</v>
       </c>
-      <c r="J5" s="14">
-        <f xml:space="preserve"> G5 * H5</f>
+      <c r="J5" s="13">
+        <f xml:space="preserve"> I5 * H5</f>
         <v>90</v>
       </c>
       <c r="K5" s="3">
@@ -1227,22 +1260,22 @@
       <c r="D6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="9">
-        <v>0</v>
-      </c>
-      <c r="G6" s="9">
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
         <v>36</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="9">
         <v>0.6</v>
       </c>
       <c r="I6" s="8">
         <v>36</v>
       </c>
-      <c r="J6" s="15">
+      <c r="J6" s="14">
         <f xml:space="preserve"> G6 * H6</f>
         <v>21.599999999999998</v>
       </c>
@@ -1256,22 +1289,22 @@
       <c r="D7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="9">
+      <c r="E7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="4">
         <v>100</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="4">
         <v>460</v>
       </c>
-      <c r="H7" s="10">
-        <v>1</v>
-      </c>
-      <c r="I7" s="9">
+      <c r="H7" s="9">
+        <v>1</v>
+      </c>
+      <c r="I7" s="4">
         <v>368.4</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="14">
         <f xml:space="preserve"> I7</f>
         <v>368.4</v>
       </c>
@@ -1285,22 +1318,22 @@
       <c r="D8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="9">
+      <c r="E8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="4">
         <v>100</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="4">
         <v>460</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="9">
         <v>1</v>
       </c>
       <c r="I8" s="8">
         <v>0</v>
       </c>
-      <c r="J8" s="15">
+      <c r="J8" s="14">
         <f t="shared" ref="J8:J10" si="1" xml:space="preserve"> I8</f>
         <v>0</v>
       </c>
@@ -1314,22 +1347,22 @@
       <c r="D9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="9">
+      <c r="E9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="4">
         <v>40</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="4">
         <v>210</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="9">
         <v>1</v>
       </c>
       <c r="I9" s="8">
         <v>0</v>
       </c>
-      <c r="J9" s="15">
+      <c r="J9" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1340,25 +1373,25 @@
     </row>
     <row r="10" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="4"/>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="12">
-        <v>0</v>
-      </c>
-      <c r="G10" s="12">
+      <c r="F10" s="11">
+        <v>0</v>
+      </c>
+      <c r="G10" s="11">
         <v>16</v>
       </c>
-      <c r="H10" s="13">
-        <v>1</v>
-      </c>
-      <c r="I10" s="11">
-        <v>0</v>
-      </c>
-      <c r="J10" s="15">
+      <c r="H10" s="12">
+        <v>1</v>
+      </c>
+      <c r="I10" s="10">
+        <v>0</v>
+      </c>
+      <c r="J10" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1401,7 +1434,7 @@
       <c r="I13" s="4"/>
     </row>
     <row r="14" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="18" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -1448,8 +1481,8 @@
       <c r="I15" s="5">
         <v>0</v>
       </c>
-      <c r="J15" s="14">
-        <f xml:space="preserve"> G15 * H15</f>
+      <c r="J15" s="13">
+        <f xml:space="preserve"> I15 * H15</f>
         <v>0</v>
       </c>
       <c r="K15" s="3">
@@ -1462,23 +1495,23 @@
       <c r="D16" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="9">
-        <v>0</v>
-      </c>
-      <c r="G16" s="9">
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4">
         <v>36</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H16" s="9">
         <v>0</v>
       </c>
       <c r="I16" s="8">
         <v>0</v>
       </c>
-      <c r="J16" s="15">
-        <f xml:space="preserve"> G16 * H16</f>
+      <c r="J16" s="14">
+        <f xml:space="preserve"> I16 * H16</f>
         <v>0</v>
       </c>
       <c r="K16" s="3">
@@ -1491,22 +1524,22 @@
       <c r="D17" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="9">
+      <c r="E17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="4">
         <v>100</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="4">
         <v>460</v>
       </c>
-      <c r="H17" s="10">
-        <v>1</v>
-      </c>
-      <c r="I17" s="9">
+      <c r="H17" s="9">
+        <v>1</v>
+      </c>
+      <c r="I17" s="4">
         <v>380</v>
       </c>
-      <c r="J17" s="15">
+      <c r="J17" s="14">
         <f t="shared" ref="J17:J20" si="2" xml:space="preserve"> I17</f>
         <v>380</v>
       </c>
@@ -1520,22 +1553,22 @@
       <c r="D18" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="9">
+      <c r="E18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="4">
         <v>100</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="4">
         <v>460</v>
       </c>
-      <c r="H18" s="10">
+      <c r="H18" s="9">
         <v>1</v>
       </c>
       <c r="I18" s="8">
         <v>100</v>
       </c>
-      <c r="J18" s="15">
+      <c r="J18" s="14">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
@@ -1549,22 +1582,22 @@
       <c r="D19" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" s="9">
+      <c r="E19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="4">
         <v>40</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="4">
         <v>210</v>
       </c>
-      <c r="H19" s="10">
+      <c r="H19" s="9">
         <v>1</v>
       </c>
       <c r="I19" s="8">
         <v>0</v>
       </c>
-      <c r="J19" s="15">
+      <c r="J19" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1575,25 +1608,25 @@
     </row>
     <row r="20" spans="3:11" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="4"/>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F20" s="12">
-        <v>0</v>
-      </c>
-      <c r="G20" s="12">
+      <c r="F20" s="11">
+        <v>0</v>
+      </c>
+      <c r="G20" s="11">
         <v>16</v>
       </c>
-      <c r="H20" s="13">
-        <v>1</v>
-      </c>
-      <c r="I20" s="11">
-        <v>0</v>
-      </c>
-      <c r="J20" s="15">
+      <c r="H20" s="12">
+        <v>1</v>
+      </c>
+      <c r="I20" s="10">
+        <v>0</v>
+      </c>
+      <c r="J20" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1603,7 +1636,7 @@
       </c>
     </row>
     <row r="21" spans="3:11" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="9"/>
+      <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
@@ -1618,7 +1651,7 @@
       </c>
     </row>
     <row r="22" spans="3:11" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="9"/>
+      <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -1628,7 +1661,7 @@
       <c r="J22" s="4"/>
     </row>
     <row r="23" spans="3:11" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="9"/>
+      <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
@@ -1638,7 +1671,7 @@
       <c r="J23" s="4"/>
     </row>
     <row r="24" spans="3:11" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="19" t="s">
+      <c r="C24" s="18" t="s">
         <v>3</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -1685,8 +1718,8 @@
       <c r="I25" s="5">
         <v>150</v>
       </c>
-      <c r="J25" s="14">
-        <f xml:space="preserve"> G25 * H25</f>
+      <c r="J25" s="13">
+        <f xml:space="preserve"> I25 * H25</f>
         <v>90</v>
       </c>
       <c r="K25" s="3">
@@ -1699,23 +1732,23 @@
       <c r="D26" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="E26" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F26" s="9">
-        <v>0</v>
-      </c>
-      <c r="G26" s="9">
+      <c r="F26" s="4">
+        <v>0</v>
+      </c>
+      <c r="G26" s="4">
         <v>36</v>
       </c>
-      <c r="H26" s="10">
+      <c r="H26" s="9">
         <v>0.6</v>
       </c>
       <c r="I26" s="8">
         <v>36</v>
       </c>
-      <c r="J26" s="15">
-        <f xml:space="preserve"> G26 * H26</f>
+      <c r="J26" s="14">
+        <f xml:space="preserve"> I26 * H26</f>
         <v>21.599999999999998</v>
       </c>
       <c r="K26" s="3">
@@ -1728,22 +1761,22 @@
       <c r="D27" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E27" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F27" s="9">
+      <c r="E27" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="4">
         <v>100</v>
       </c>
-      <c r="G27" s="9">
+      <c r="G27" s="4">
         <v>460</v>
       </c>
-      <c r="H27" s="10">
-        <v>1</v>
-      </c>
-      <c r="I27" s="9">
+      <c r="H27" s="9">
+        <v>1</v>
+      </c>
+      <c r="I27" s="4">
         <v>460</v>
       </c>
-      <c r="J27" s="15">
+      <c r="J27" s="14">
         <f t="shared" ref="J27:J30" si="4" xml:space="preserve"> I27</f>
         <v>460</v>
       </c>
@@ -1757,22 +1790,22 @@
       <c r="D28" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E28" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F28" s="9">
+      <c r="E28" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="4">
         <v>100</v>
       </c>
-      <c r="G28" s="9">
+      <c r="G28" s="4">
         <v>460</v>
       </c>
-      <c r="H28" s="10">
+      <c r="H28" s="9">
         <v>1</v>
       </c>
       <c r="I28" s="8">
         <v>338.4</v>
       </c>
-      <c r="J28" s="15">
+      <c r="J28" s="14">
         <f t="shared" si="4"/>
         <v>338.4</v>
       </c>
@@ -1786,22 +1819,22 @@
       <c r="D29" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29" s="9">
+      <c r="E29" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="4">
         <v>40</v>
       </c>
-      <c r="G29" s="9">
+      <c r="G29" s="4">
         <v>210</v>
       </c>
-      <c r="H29" s="10">
+      <c r="H29" s="9">
         <v>1</v>
       </c>
       <c r="I29" s="8">
         <v>0</v>
       </c>
-      <c r="J29" s="15">
+      <c r="J29" s="14">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -1812,25 +1845,25 @@
     </row>
     <row r="30" spans="3:11" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="4"/>
-      <c r="D30" s="11" t="s">
+      <c r="D30" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="E30" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F30" s="12">
-        <v>0</v>
-      </c>
-      <c r="G30" s="12">
+      <c r="F30" s="11">
+        <v>0</v>
+      </c>
+      <c r="G30" s="11">
         <v>16</v>
       </c>
-      <c r="H30" s="13">
-        <v>1</v>
-      </c>
-      <c r="I30" s="11">
-        <v>0</v>
-      </c>
-      <c r="J30" s="15">
+      <c r="H30" s="12">
+        <v>1</v>
+      </c>
+      <c r="I30" s="10">
+        <v>0</v>
+      </c>
+      <c r="J30" s="14">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -1856,7 +1889,7 @@
     </row>
     <row r="32" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="19" t="s">
+      <c r="C33" s="18" t="s">
         <v>26</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -1904,8 +1937,8 @@
       <c r="I34" s="5">
         <v>0</v>
       </c>
-      <c r="J34" s="14">
-        <f xml:space="preserve"> G34 * H34</f>
+      <c r="J34" s="13">
+        <f xml:space="preserve"> I34 * H34</f>
         <v>0</v>
       </c>
       <c r="K34" s="3">
@@ -1919,23 +1952,23 @@
       <c r="D35" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E35" s="9" t="s">
+      <c r="E35" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F35" s="9">
-        <v>0</v>
-      </c>
-      <c r="G35" s="9">
+      <c r="F35" s="4">
+        <v>0</v>
+      </c>
+      <c r="G35" s="4">
         <v>36</v>
       </c>
-      <c r="H35" s="10">
+      <c r="H35" s="9">
         <v>0</v>
       </c>
       <c r="I35" s="8">
         <v>0</v>
       </c>
-      <c r="J35" s="15">
-        <f xml:space="preserve"> G35 * H35</f>
+      <c r="J35" s="14">
+        <f xml:space="preserve"> I35 * H35</f>
         <v>0</v>
       </c>
       <c r="K35" s="3">
@@ -1949,22 +1982,22 @@
       <c r="D36" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E36" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F36" s="9">
+      <c r="E36" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="4">
         <v>100</v>
       </c>
-      <c r="G36" s="9">
+      <c r="G36" s="4">
         <v>460</v>
       </c>
-      <c r="H36" s="10">
-        <v>1</v>
-      </c>
-      <c r="I36" s="9">
-        <v>0</v>
-      </c>
-      <c r="J36" s="15">
+      <c r="H36" s="9">
+        <v>1</v>
+      </c>
+      <c r="I36" s="4">
+        <v>0</v>
+      </c>
+      <c r="J36" s="14">
         <f t="shared" ref="J36:J39" si="6" xml:space="preserve"> I36</f>
         <v>0</v>
       </c>
@@ -1979,22 +2012,22 @@
       <c r="D37" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E37" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F37" s="9">
+      <c r="E37" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="4">
         <v>100</v>
       </c>
-      <c r="G37" s="9">
+      <c r="G37" s="4">
         <v>460</v>
       </c>
-      <c r="H37" s="10">
+      <c r="H37" s="9">
         <v>1</v>
       </c>
       <c r="I37" s="8">
         <v>0</v>
       </c>
-      <c r="J37" s="15">
+      <c r="J37" s="14">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -2009,22 +2042,22 @@
       <c r="D38" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E38" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F38" s="9">
+      <c r="E38" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="4">
         <v>40</v>
       </c>
-      <c r="G38" s="9">
+      <c r="G38" s="4">
         <v>210</v>
       </c>
-      <c r="H38" s="10">
+      <c r="H38" s="9">
         <v>1</v>
       </c>
       <c r="I38" s="8">
         <v>50</v>
       </c>
-      <c r="J38" s="15">
+      <c r="J38" s="14">
         <f t="shared" si="6"/>
         <v>50</v>
       </c>
@@ -2036,25 +2069,25 @@
     </row>
     <row r="39" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C39" s="4"/>
-      <c r="D39" s="11" t="s">
+      <c r="D39" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E39" s="12" t="s">
+      <c r="E39" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F39" s="12">
-        <v>0</v>
-      </c>
-      <c r="G39" s="12">
+      <c r="F39" s="11">
+        <v>0</v>
+      </c>
+      <c r="G39" s="11">
         <v>16</v>
       </c>
-      <c r="H39" s="13">
-        <v>1</v>
-      </c>
-      <c r="I39" s="11">
-        <v>0</v>
-      </c>
-      <c r="J39" s="15">
+      <c r="H39" s="12">
+        <v>1</v>
+      </c>
+      <c r="I39" s="10">
+        <v>0</v>
+      </c>
+      <c r="J39" s="14">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -2065,7 +2098,7 @@
       <c r="L39" s="4"/>
     </row>
     <row r="40" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C40" s="9"/>
+      <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
@@ -2080,6 +2113,1379 @@
       </c>
       <c r="K40" s="3"/>
     </row>
+    <row r="41" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L42" s="4"/>
+    </row>
+    <row r="43" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C43" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F43" s="6">
+        <v>0</v>
+      </c>
+      <c r="G43" s="6">
+        <v>150</v>
+      </c>
+      <c r="H43" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="I43" s="5">
+        <v>150</v>
+      </c>
+      <c r="J43" s="13">
+        <f xml:space="preserve"> I43 * H43</f>
+        <v>90</v>
+      </c>
+      <c r="K43" s="3">
+        <f>SUM(J43:J48)</f>
+        <v>152</v>
+      </c>
+      <c r="L43" s="4"/>
+    </row>
+    <row r="44" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C44" s="4"/>
+      <c r="D44" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F44" s="4">
+        <v>0</v>
+      </c>
+      <c r="G44" s="4">
+        <v>36</v>
+      </c>
+      <c r="H44" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="I44" s="8">
+        <v>36</v>
+      </c>
+      <c r="J44" s="14">
+        <f xml:space="preserve"> I44 * H44</f>
+        <v>21.599999999999998</v>
+      </c>
+      <c r="K44" s="3">
+        <f xml:space="preserve"> K43 - J43</f>
+        <v>62</v>
+      </c>
+      <c r="L44" s="4"/>
+    </row>
+    <row r="45" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C45" s="4"/>
+      <c r="D45" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45" s="4">
+        <v>100</v>
+      </c>
+      <c r="G45" s="4">
+        <v>460</v>
+      </c>
+      <c r="H45" s="9">
+        <v>1</v>
+      </c>
+      <c r="I45" s="4">
+        <v>0</v>
+      </c>
+      <c r="J45" s="14">
+        <f t="shared" ref="J45:J48" si="8" xml:space="preserve"> I45</f>
+        <v>0</v>
+      </c>
+      <c r="K45" s="3">
+        <f t="shared" ref="K45:K48" si="9" xml:space="preserve"> K44 - J44</f>
+        <v>40.400000000000006</v>
+      </c>
+      <c r="L45" s="4"/>
+    </row>
+    <row r="46" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C46" s="4"/>
+      <c r="D46" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46" s="4">
+        <v>100</v>
+      </c>
+      <c r="G46" s="4">
+        <v>460</v>
+      </c>
+      <c r="H46" s="9">
+        <v>1</v>
+      </c>
+      <c r="I46" s="8">
+        <v>0</v>
+      </c>
+      <c r="J46" s="14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K46" s="3">
+        <f t="shared" si="9"/>
+        <v>40.400000000000006</v>
+      </c>
+      <c r="L46" s="4"/>
+    </row>
+    <row r="47" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C47" s="4"/>
+      <c r="D47" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F47" s="4">
+        <v>40</v>
+      </c>
+      <c r="G47" s="4">
+        <v>210</v>
+      </c>
+      <c r="H47" s="9">
+        <v>1</v>
+      </c>
+      <c r="I47" s="8">
+        <v>40.4</v>
+      </c>
+      <c r="J47" s="14">
+        <f t="shared" si="8"/>
+        <v>40.4</v>
+      </c>
+      <c r="K47" s="3">
+        <f t="shared" si="9"/>
+        <v>40.400000000000006</v>
+      </c>
+      <c r="L47" s="4"/>
+    </row>
+    <row r="48" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C48" s="4"/>
+      <c r="D48" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48" s="11">
+        <v>0</v>
+      </c>
+      <c r="G48" s="11">
+        <v>16</v>
+      </c>
+      <c r="H48" s="12">
+        <v>1</v>
+      </c>
+      <c r="I48" s="10">
+        <v>0</v>
+      </c>
+      <c r="J48" s="14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K48" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L48" s="4"/>
+    </row>
+    <row r="49" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J49" s="2">
+        <f xml:space="preserve"> SUM(J43:J48)</f>
+        <v>152</v>
+      </c>
+      <c r="L49" s="4"/>
+    </row>
+    <row r="50" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="4"/>
+    </row>
+    <row r="51" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C51" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L51" s="4"/>
+    </row>
+    <row r="52" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C52" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F52" s="6">
+        <v>0</v>
+      </c>
+      <c r="G52" s="6">
+        <v>150</v>
+      </c>
+      <c r="H52" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="I52" s="5">
+        <v>150</v>
+      </c>
+      <c r="J52" s="13">
+        <f xml:space="preserve"> I52 * H52</f>
+        <v>90</v>
+      </c>
+      <c r="K52" s="3">
+        <f>SUM(J52:J57)</f>
+        <v>183.6</v>
+      </c>
+      <c r="L52" s="4"/>
+    </row>
+    <row r="53" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C53" s="4"/>
+      <c r="D53" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F53" s="4">
+        <v>0</v>
+      </c>
+      <c r="G53" s="4">
+        <v>36</v>
+      </c>
+      <c r="H53" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="I53" s="8">
+        <v>36</v>
+      </c>
+      <c r="J53" s="14">
+        <f xml:space="preserve"> I53 * H53</f>
+        <v>21.599999999999998</v>
+      </c>
+      <c r="K53" s="3">
+        <f xml:space="preserve"> K52 - J52</f>
+        <v>93.6</v>
+      </c>
+      <c r="L53" s="4"/>
+    </row>
+    <row r="54" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C54" s="4"/>
+      <c r="D54" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54" s="4">
+        <v>100</v>
+      </c>
+      <c r="G54" s="4">
+        <v>460</v>
+      </c>
+      <c r="H54" s="9">
+        <v>1</v>
+      </c>
+      <c r="I54" s="4">
+        <v>0</v>
+      </c>
+      <c r="J54" s="14">
+        <f t="shared" ref="J54:J57" si="10" xml:space="preserve"> I54</f>
+        <v>0</v>
+      </c>
+      <c r="K54" s="3">
+        <f t="shared" ref="K54:K58" si="11" xml:space="preserve"> K53 - J53</f>
+        <v>72</v>
+      </c>
+      <c r="L54" s="4"/>
+    </row>
+    <row r="55" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C55" s="4"/>
+      <c r="D55" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" s="4">
+        <v>100</v>
+      </c>
+      <c r="G55" s="4">
+        <v>460</v>
+      </c>
+      <c r="H55" s="9">
+        <v>1</v>
+      </c>
+      <c r="I55" s="8">
+        <v>0</v>
+      </c>
+      <c r="J55" s="14">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K55" s="3">
+        <f t="shared" si="11"/>
+        <v>72</v>
+      </c>
+      <c r="L55" s="4"/>
+    </row>
+    <row r="56" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C56" s="4"/>
+      <c r="D56" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" s="4">
+        <v>40</v>
+      </c>
+      <c r="G56" s="4">
+        <v>60</v>
+      </c>
+      <c r="H56" s="9">
+        <v>1</v>
+      </c>
+      <c r="I56" s="8">
+        <v>60</v>
+      </c>
+      <c r="J56" s="14">
+        <f t="shared" si="10"/>
+        <v>60</v>
+      </c>
+      <c r="K56" s="3">
+        <f t="shared" si="11"/>
+        <v>72</v>
+      </c>
+      <c r="L56" s="4"/>
+    </row>
+    <row r="57" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C57" s="4"/>
+      <c r="D57" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F57" s="11">
+        <v>0</v>
+      </c>
+      <c r="G57" s="11">
+        <v>16</v>
+      </c>
+      <c r="H57" s="12">
+        <v>1</v>
+      </c>
+      <c r="I57" s="10">
+        <v>12</v>
+      </c>
+      <c r="J57" s="14">
+        <f t="shared" si="10"/>
+        <v>12</v>
+      </c>
+      <c r="K57" s="3">
+        <f t="shared" si="11"/>
+        <v>12</v>
+      </c>
+      <c r="L57" s="4"/>
+    </row>
+    <row r="58" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J58" s="2">
+        <f xml:space="preserve"> SUM(J52:J57)</f>
+        <v>183.6</v>
+      </c>
+      <c r="K58" s="3">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="L58" s="4"/>
+    </row>
+    <row r="59" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C60" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L60" s="4"/>
+    </row>
+    <row r="61" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C61" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F61" s="6">
+        <v>0</v>
+      </c>
+      <c r="G61" s="6">
+        <v>150</v>
+      </c>
+      <c r="H61" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="I61" s="5">
+        <v>150</v>
+      </c>
+      <c r="J61" s="13">
+        <f xml:space="preserve"> I61 * H61</f>
+        <v>90</v>
+      </c>
+      <c r="K61" s="3">
+        <f>SUM(J61:J66)</f>
+        <v>173.6</v>
+      </c>
+      <c r="L61" s="4"/>
+    </row>
+    <row r="62" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C62" s="4"/>
+      <c r="D62" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F62" s="4">
+        <v>0</v>
+      </c>
+      <c r="G62" s="4">
+        <v>36</v>
+      </c>
+      <c r="H62" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="I62" s="8">
+        <v>36</v>
+      </c>
+      <c r="J62" s="14">
+        <f xml:space="preserve"> I62 * H62</f>
+        <v>21.599999999999998</v>
+      </c>
+      <c r="K62" s="3">
+        <f xml:space="preserve"> K61 - J61</f>
+        <v>83.6</v>
+      </c>
+      <c r="L62" s="4"/>
+    </row>
+    <row r="63" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C63" s="4"/>
+      <c r="D63" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F63" s="4">
+        <v>100</v>
+      </c>
+      <c r="G63" s="4">
+        <v>460</v>
+      </c>
+      <c r="H63" s="9">
+        <v>1</v>
+      </c>
+      <c r="I63" s="4">
+        <v>0</v>
+      </c>
+      <c r="J63" s="14">
+        <f t="shared" ref="J63:J66" si="12" xml:space="preserve"> I63</f>
+        <v>0</v>
+      </c>
+      <c r="K63" s="3">
+        <f t="shared" ref="K63:K67" si="13" xml:space="preserve"> K62 - J62</f>
+        <v>62</v>
+      </c>
+      <c r="L63" s="4"/>
+    </row>
+    <row r="64" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C64" s="4"/>
+      <c r="D64" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F64" s="4">
+        <v>100</v>
+      </c>
+      <c r="G64" s="4">
+        <v>460</v>
+      </c>
+      <c r="H64" s="9">
+        <v>1</v>
+      </c>
+      <c r="I64" s="8">
+        <v>0</v>
+      </c>
+      <c r="J64" s="14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K64" s="3">
+        <f t="shared" si="13"/>
+        <v>62</v>
+      </c>
+      <c r="L64" s="4"/>
+    </row>
+    <row r="65" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C65" s="4"/>
+      <c r="D65" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F65" s="4">
+        <v>40</v>
+      </c>
+      <c r="G65" s="4">
+        <v>60</v>
+      </c>
+      <c r="H65" s="9">
+        <v>1</v>
+      </c>
+      <c r="I65" s="8">
+        <v>60</v>
+      </c>
+      <c r="J65" s="14">
+        <f t="shared" si="12"/>
+        <v>60</v>
+      </c>
+      <c r="K65" s="3">
+        <f t="shared" si="13"/>
+        <v>62</v>
+      </c>
+      <c r="L65" s="4"/>
+    </row>
+    <row r="66" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C66" s="4"/>
+      <c r="D66" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E66" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F66" s="11">
+        <v>0</v>
+      </c>
+      <c r="G66" s="11">
+        <v>16</v>
+      </c>
+      <c r="H66" s="12">
+        <v>1</v>
+      </c>
+      <c r="I66" s="10">
+        <v>2</v>
+      </c>
+      <c r="J66" s="14">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="K66" s="3">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="L66" s="4"/>
+    </row>
+    <row r="67" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="4"/>
+      <c r="G67" s="4"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J67" s="2">
+        <f xml:space="preserve"> SUM(J61:J66)</f>
+        <v>173.6</v>
+      </c>
+      <c r="K67" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="L67" s="4"/>
+    </row>
+    <row r="69" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="70" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C70" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I70" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J70" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L70" s="4"/>
+    </row>
+    <row r="71" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C71" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F71" s="6">
+        <v>0</v>
+      </c>
+      <c r="G71" s="6">
+        <v>150</v>
+      </c>
+      <c r="H71" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="I71" s="5">
+        <v>0</v>
+      </c>
+      <c r="J71" s="13">
+        <f xml:space="preserve"> I71 * H71</f>
+        <v>0</v>
+      </c>
+      <c r="K71" s="3">
+        <f>SUM(J71:J76)</f>
+        <v>71.599999999999994</v>
+      </c>
+      <c r="L71" s="4"/>
+    </row>
+    <row r="72" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C72" s="4"/>
+      <c r="D72" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F72" s="4">
+        <v>0</v>
+      </c>
+      <c r="G72" s="4">
+        <v>36</v>
+      </c>
+      <c r="H72" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="I72" s="8">
+        <v>36</v>
+      </c>
+      <c r="J72" s="14">
+        <f xml:space="preserve"> I72 * H72</f>
+        <v>21.599999999999998</v>
+      </c>
+      <c r="K72" s="3">
+        <f xml:space="preserve"> K71 - J71</f>
+        <v>71.599999999999994</v>
+      </c>
+      <c r="L72" s="4"/>
+    </row>
+    <row r="73" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C73" s="4"/>
+      <c r="D73" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F73" s="4">
+        <v>100</v>
+      </c>
+      <c r="G73" s="4">
+        <v>460</v>
+      </c>
+      <c r="H73" s="9">
+        <v>1</v>
+      </c>
+      <c r="I73" s="4">
+        <v>0</v>
+      </c>
+      <c r="J73" s="14">
+        <f t="shared" ref="J73:J76" si="14" xml:space="preserve"> I73</f>
+        <v>0</v>
+      </c>
+      <c r="K73" s="3">
+        <f t="shared" ref="K73:K77" si="15" xml:space="preserve"> K72 - J72</f>
+        <v>50</v>
+      </c>
+      <c r="L73" s="4"/>
+    </row>
+    <row r="74" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C74" s="4"/>
+      <c r="D74" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F74" s="4">
+        <v>100</v>
+      </c>
+      <c r="G74" s="4">
+        <v>460</v>
+      </c>
+      <c r="H74" s="9">
+        <v>1</v>
+      </c>
+      <c r="I74" s="8">
+        <v>0</v>
+      </c>
+      <c r="J74" s="14">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="K74" s="3">
+        <f t="shared" si="15"/>
+        <v>50</v>
+      </c>
+      <c r="L74" s="4"/>
+    </row>
+    <row r="75" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C75" s="4"/>
+      <c r="D75" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F75" s="4">
+        <v>40</v>
+      </c>
+      <c r="G75" s="4">
+        <v>60</v>
+      </c>
+      <c r="H75" s="9">
+        <v>1</v>
+      </c>
+      <c r="I75" s="8">
+        <v>50</v>
+      </c>
+      <c r="J75" s="14">
+        <f t="shared" si="14"/>
+        <v>50</v>
+      </c>
+      <c r="K75" s="3">
+        <f t="shared" si="15"/>
+        <v>50</v>
+      </c>
+      <c r="L75" s="4"/>
+    </row>
+    <row r="76" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C76" s="4"/>
+      <c r="D76" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F76" s="11">
+        <v>0</v>
+      </c>
+      <c r="G76" s="11">
+        <v>16</v>
+      </c>
+      <c r="H76" s="12">
+        <v>1</v>
+      </c>
+      <c r="I76" s="10">
+        <v>0</v>
+      </c>
+      <c r="J76" s="14">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="K76" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="L76" s="4"/>
+    </row>
+    <row r="77" spans="3:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C77" s="4"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
+      <c r="G77" s="4"/>
+      <c r="H77" s="4"/>
+      <c r="I77" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J77" s="2">
+        <f xml:space="preserve"> SUM(J71:J76)</f>
+        <v>71.599999999999994</v>
+      </c>
+      <c r="K77" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="L77" s="4"/>
+    </row>
+    <row r="78" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="79" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C79" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J79" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K79" s="3"/>
+    </row>
+    <row r="80" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C80" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F80" s="6">
+        <v>0</v>
+      </c>
+      <c r="G80" s="6">
+        <v>150</v>
+      </c>
+      <c r="H80" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="I80" s="5">
+        <v>0</v>
+      </c>
+      <c r="J80" s="13">
+        <f xml:space="preserve"> I80 * H80</f>
+        <v>0</v>
+      </c>
+      <c r="K80" s="3">
+        <f>SUM(J80:J85)</f>
+        <v>86.6</v>
+      </c>
+    </row>
+    <row r="81" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C81" s="4"/>
+      <c r="D81" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F81" s="4">
+        <v>0</v>
+      </c>
+      <c r="G81" s="4">
+        <v>36</v>
+      </c>
+      <c r="H81" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="I81" s="8">
+        <v>36</v>
+      </c>
+      <c r="J81" s="14">
+        <f xml:space="preserve"> I81 * H81</f>
+        <v>21.599999999999998</v>
+      </c>
+      <c r="K81" s="3">
+        <f xml:space="preserve"> K80 - J80</f>
+        <v>86.6</v>
+      </c>
+    </row>
+    <row r="82" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C82" s="4"/>
+      <c r="D82" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F82" s="4">
+        <v>100</v>
+      </c>
+      <c r="G82" s="4">
+        <v>460</v>
+      </c>
+      <c r="H82" s="9">
+        <v>1</v>
+      </c>
+      <c r="I82" s="4">
+        <v>0</v>
+      </c>
+      <c r="J82" s="14">
+        <f t="shared" ref="J82:J85" si="16" xml:space="preserve"> I82</f>
+        <v>0</v>
+      </c>
+      <c r="K82" s="3">
+        <f t="shared" ref="K82:K86" si="17" xml:space="preserve"> K81 - J81</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="83" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C83" s="4"/>
+      <c r="D83" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F83" s="4">
+        <v>100</v>
+      </c>
+      <c r="G83" s="4">
+        <v>460</v>
+      </c>
+      <c r="H83" s="9">
+        <v>1</v>
+      </c>
+      <c r="I83" s="8">
+        <v>0</v>
+      </c>
+      <c r="J83" s="14">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="K83" s="3">
+        <f t="shared" si="17"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="84" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C84" s="4"/>
+      <c r="D84" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F84" s="4">
+        <v>40</v>
+      </c>
+      <c r="G84" s="4">
+        <v>60</v>
+      </c>
+      <c r="H84" s="9">
+        <v>1</v>
+      </c>
+      <c r="I84" s="8">
+        <v>55</v>
+      </c>
+      <c r="J84" s="14">
+        <f t="shared" si="16"/>
+        <v>55</v>
+      </c>
+      <c r="K84" s="3">
+        <f t="shared" si="17"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="85" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C85" s="4"/>
+      <c r="D85" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E85" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F85" s="11">
+        <v>10</v>
+      </c>
+      <c r="G85" s="11">
+        <v>16</v>
+      </c>
+      <c r="H85" s="12">
+        <v>1</v>
+      </c>
+      <c r="I85" s="10">
+        <v>10</v>
+      </c>
+      <c r="J85" s="14">
+        <f t="shared" si="16"/>
+        <v>10</v>
+      </c>
+      <c r="K85" s="3">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C86" s="4"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="4"/>
+      <c r="G86" s="4"/>
+      <c r="H86" s="4"/>
+      <c r="I86" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J86" s="2">
+        <f xml:space="preserve"> SUM(J80:J85)</f>
+        <v>86.6</v>
+      </c>
+      <c r="K86" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="88" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C88" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I88" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J88" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K88" s="3"/>
+    </row>
+    <row r="89" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C89" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E89" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F89" s="6">
+        <v>0</v>
+      </c>
+      <c r="G89" s="6">
+        <v>150</v>
+      </c>
+      <c r="H89" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="I89" s="5">
+        <v>0</v>
+      </c>
+      <c r="J89" s="13">
+        <f xml:space="preserve"> I89 * H89</f>
+        <v>0</v>
+      </c>
+      <c r="K89" s="3">
+        <f>SUM(J89:J94)</f>
+        <v>31.599999999999998</v>
+      </c>
+    </row>
+    <row r="90" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C90" s="4"/>
+      <c r="D90" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F90" s="4">
+        <v>0</v>
+      </c>
+      <c r="G90" s="4">
+        <v>36</v>
+      </c>
+      <c r="H90" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="I90" s="8">
+        <v>36</v>
+      </c>
+      <c r="J90" s="14">
+        <f xml:space="preserve"> I90 * H90</f>
+        <v>21.599999999999998</v>
+      </c>
+      <c r="K90" s="3">
+        <f xml:space="preserve"> K89 - J89</f>
+        <v>31.599999999999998</v>
+      </c>
+    </row>
+    <row r="91" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C91" s="4"/>
+      <c r="D91" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F91" s="4">
+        <v>100</v>
+      </c>
+      <c r="G91" s="4">
+        <v>460</v>
+      </c>
+      <c r="H91" s="9">
+        <v>1</v>
+      </c>
+      <c r="I91" s="4">
+        <v>0</v>
+      </c>
+      <c r="J91" s="14">
+        <f t="shared" ref="J91:J94" si="18" xml:space="preserve"> I91</f>
+        <v>0</v>
+      </c>
+      <c r="K91" s="3">
+        <f t="shared" ref="K91:K95" si="19" xml:space="preserve"> K90 - J90</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C92" s="4"/>
+      <c r="D92" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F92" s="4">
+        <v>100</v>
+      </c>
+      <c r="G92" s="4">
+        <v>460</v>
+      </c>
+      <c r="H92" s="9">
+        <v>1</v>
+      </c>
+      <c r="I92" s="8">
+        <v>0</v>
+      </c>
+      <c r="J92" s="14">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K92" s="3">
+        <f t="shared" si="19"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C93" s="4"/>
+      <c r="D93" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F93" s="4">
+        <v>40</v>
+      </c>
+      <c r="G93" s="4">
+        <v>60</v>
+      </c>
+      <c r="H93" s="9">
+        <v>1</v>
+      </c>
+      <c r="I93" s="8">
+        <v>0</v>
+      </c>
+      <c r="J93" s="14">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="K93" s="3">
+        <f t="shared" si="19"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C94" s="4"/>
+      <c r="D94" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E94" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F94" s="11">
+        <v>0</v>
+      </c>
+      <c r="G94" s="11">
+        <v>16</v>
+      </c>
+      <c r="H94" s="12">
+        <v>1</v>
+      </c>
+      <c r="I94" s="10">
+        <v>10</v>
+      </c>
+      <c r="J94" s="14">
+        <f t="shared" si="18"/>
+        <v>10</v>
+      </c>
+      <c r="K94" s="3">
+        <f t="shared" si="19"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="95" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C95" s="4"/>
+      <c r="D95" s="4"/>
+      <c r="E95" s="4"/>
+      <c r="F95" s="4"/>
+      <c r="G95" s="4"/>
+      <c r="H95" s="4"/>
+      <c r="I95" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J95" s="2">
+        <f xml:space="preserve"> SUM(J89:J94)</f>
+        <v>31.599999999999998</v>
+      </c>
+      <c r="K95" s="3">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>